<commit_message>
Adding Processed Lanz GSEA with H+S files
</commit_message>
<xml_diff>
--- a/Datasets for KS Input/Smita List of Curated Datasets for KS Input.xlsx
+++ b/Datasets for KS Input/Smita List of Curated Datasets for KS Input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smitasahay/Desktop/PhD/Projects/Ketosis Project/ketosis_project/Datasets for KS Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smitasahay/Desktop/PhD/Projects/Ketosis BI Paper/ketosis_project/Datasets for KS Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A25801-B2E1-774D-9A2B-D5975E93C1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C4A32E-67E6-4842-9FD8-617D1645E9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="1780" windowWidth="30600" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31600" yWindow="2020" windowWidth="30600" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RNA-Seq Data" sheetId="1" r:id="rId1"/>
@@ -1358,7 +1358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="68" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
@@ -1902,10 +1902,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB27637-4313-A342-BACD-83E963CE018B}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView zoomScale="65" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2102,7 +2102,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="152">
+    <row r="5" spans="1:15" ht="133">
       <c r="A5" s="26">
         <v>200062105</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="95">
+    <row r="6" spans="1:15" ht="80">
       <c r="A6" s="26">
         <v>200001829</v>
       </c>
@@ -2557,6 +2557,9 @@
       <c r="L19" s="16"/>
       <c r="M19" s="35"/>
       <c r="N19" s="26"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="C24"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3394,21 +3397,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034B2111F16753748B07B8B2A03D6410C" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c54d6f00b4000a0e053db110112d707">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dba05a22-d3d4-4800-8353-2deabbd0fb1d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca2460e8561fc9eb4be35c86fe727f91" ns3:_="">
     <xsd:import namespace="dba05a22-d3d4-4800-8353-2deabbd0fb1d"/>
@@ -3572,24 +3560,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F26D0B6-AFD8-4D33-AA54-AAEB31DB979E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2B9A09B-0EA7-4ECB-B6A7-B701DD5D6BD4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{833422F9-EA10-412F-A3DB-70A7B71D2D3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3605,4 +3591,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2B9A09B-0EA7-4ECB-B6A7-B701DD5D6BD4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F26D0B6-AFD8-4D33-AA54-AAEB31DB979E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding GSEA Ramaker + Lanz analysis files
</commit_message>
<xml_diff>
--- a/Datasets for KS Input/Smita List of Curated Datasets for KS Input.xlsx
+++ b/Datasets for KS Input/Smita List of Curated Datasets for KS Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smitasahay/Desktop/PhD/Projects/Ketosis BI Paper/ketosis_project/Datasets for KS Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C4A32E-67E6-4842-9FD8-617D1645E9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F5298D-02D0-1949-B229-66A1DE33222C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31600" yWindow="2020" windowWidth="30600" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27200" windowHeight="16100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RNA-Seq Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="241">
   <si>
     <t>Pubmed ID</t>
   </si>
@@ -708,13 +708,83 @@
   </si>
   <si>
     <t>Processed (DEG w Gene Name)</t>
+  </si>
+  <si>
+    <t>GSE53987</t>
+  </si>
+  <si>
+    <t>BIPOLAR</t>
+  </si>
+  <si>
+    <t>GPL570: [HG-U133_Plus_2] Affymetrix Human Genome U133 Plus 2.0 Array</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <r>
+      <t>Yes (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>6 total comparisons</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve"> for male and female for 3 different brain regions)</t>
+    </r>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Missing Gene IDs filled in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ncbi.nlm.nih.gov/geo/query/acc.cgi?acc=GSE53987  </t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/31123247/</t>
+  </si>
+  <si>
+    <t>Lanz TA</t>
+  </si>
+  <si>
+    <t>Separate folder sent on KS Slack: Lanz DGEs --&gt; BPD</t>
+  </si>
+  <si>
+    <t>Separate folder sent on KS Slack: Lanz DGEs --&gt; SCZ</t>
+  </si>
+  <si>
+    <t>Separate folder sent on KS Slack: Lanz DGEs --&gt; MDD</t>
+  </si>
+  <si>
+    <t>PFC, Striatum, Hippocampus</t>
+  </si>
+  <si>
+    <t>Post-mortem brain tissue was collected from control subjects and well-matched subjects with schizophrenia, BPD, and MDD (n=19 from each group). RNA was isolated from hippocampus, Brodmann Area 46, and associative striatum and hybridized to U133_Plus2 Affymetrix chips. </t>
+  </si>
+  <si>
+    <t>Matched controls n=19</t>
+  </si>
+  <si>
+    <t>n=19 SCZ subjects; tissue collected from 3 brain regions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -790,30 +860,9 @@
     </font>
     <font>
       <sz val="14"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -841,8 +890,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times Roman"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Times Roman"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Times Roman"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Times Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times Roman"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times Roman"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times Roman"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -867,8 +970,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -922,12 +1037,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -995,50 +1145,111 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1432,7 +1643,7 @@
       <c r="B2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="31" t="s">
         <v>215</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -1456,17 +1667,17 @@
       <c r="J2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="38"/>
-      <c r="L2" s="30" t="s">
+      <c r="K2" s="32"/>
+      <c r="L2" s="28" t="s">
         <v>21</v>
       </c>
       <c r="M2" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="O2" s="31" t="s">
+      <c r="O2" s="29" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1477,7 +1688,7 @@
       <c r="B3" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="31" t="s">
         <v>215</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -1501,17 +1712,17 @@
       <c r="J3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="30" t="s">
+      <c r="K3" s="32"/>
+      <c r="L3" s="28" t="s">
         <v>147</v>
       </c>
       <c r="M3" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="N3" s="31" t="s">
+      <c r="N3" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="O3" s="31" t="s">
+      <c r="O3" s="29" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1522,7 +1733,7 @@
       <c r="B4" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="31" t="s">
         <v>215</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -1546,17 +1757,17 @@
       <c r="J4" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="K4" s="39"/>
-      <c r="L4" s="30" t="s">
+      <c r="K4" s="33"/>
+      <c r="L4" s="28" t="s">
         <v>202</v>
       </c>
       <c r="M4" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="N4" s="31" t="s">
+      <c r="N4" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="O4" s="31" t="s">
+      <c r="O4" s="29" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1567,7 +1778,7 @@
       <c r="B5" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="31" t="s">
         <v>215</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1591,17 +1802,17 @@
       <c r="J5" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="K5" s="39"/>
-      <c r="L5" s="30" t="s">
+      <c r="K5" s="33"/>
+      <c r="L5" s="28" t="s">
         <v>202</v>
       </c>
       <c r="M5" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="N5" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="O5" s="31" t="s">
+      <c r="O5" s="29" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1612,7 +1823,7 @@
       <c r="B6" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="31" t="s">
         <v>215</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1636,17 +1847,17 @@
       <c r="J6" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="K6" s="39"/>
-      <c r="L6" s="30" t="s">
+      <c r="K6" s="33"/>
+      <c r="L6" s="28" t="s">
         <v>202</v>
       </c>
       <c r="M6" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="O6" s="31" t="s">
+      <c r="O6" s="29" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1657,7 +1868,7 @@
       <c r="B7" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="31" t="s">
         <v>215</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1681,17 +1892,17 @@
       <c r="J7" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="K7" s="39"/>
-      <c r="L7" s="30" t="s">
+      <c r="K7" s="33"/>
+      <c r="L7" s="28" t="s">
         <v>202</v>
       </c>
       <c r="M7" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="N7" s="31" t="s">
+      <c r="N7" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="O7" s="31" t="s">
+      <c r="O7" s="29" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1706,7 +1917,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="6"/>
-      <c r="K8" s="39" t="s">
+      <c r="K8" s="33" t="s">
         <v>207</v>
       </c>
       <c r="L8" s="14"/>
@@ -1724,8 +1935,8 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="30"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="28"/>
       <c r="L9" s="14"/>
       <c r="M9" s="5"/>
       <c r="N9" s="14"/>
@@ -1741,8 +1952,8 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="30"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="28"/>
       <c r="L10" s="15"/>
       <c r="N10" s="15"/>
     </row>
@@ -1755,8 +1966,8 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="30"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="28"/>
       <c r="L11" s="15"/>
       <c r="N11" s="15"/>
     </row>
@@ -1769,8 +1980,8 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="30"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="28"/>
       <c r="L12" s="15"/>
       <c r="N12" s="15"/>
     </row>
@@ -1783,8 +1994,8 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="30"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="28"/>
       <c r="L13" s="15"/>
       <c r="N13" s="15"/>
     </row>
@@ -1797,8 +2008,8 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="30"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="28"/>
       <c r="L14" s="15"/>
       <c r="N14" s="15"/>
     </row>
@@ -1811,8 +2022,8 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="30"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="28"/>
       <c r="L15" s="15"/>
       <c r="N15" s="15"/>
     </row>
@@ -1826,8 +2037,8 @@
       <c r="G16" s="7"/>
       <c r="H16" s="10"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
       <c r="L16" s="16"/>
       <c r="N16" s="16"/>
     </row>
@@ -1841,8 +2052,8 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
       <c r="L17" s="16"/>
       <c r="N17" s="16"/>
     </row>
@@ -1856,8 +2067,8 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
       <c r="L18" s="16"/>
       <c r="N18" s="16"/>
     </row>
@@ -1871,8 +2082,8 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
       <c r="L19" s="16"/>
       <c r="N19" s="16"/>
     </row>
@@ -1904,8 +2115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB27637-4313-A342-BACD-83E963CE018B}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:D24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1914,9 +2125,9 @@
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="28.5" style="17" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" style="17" customWidth="1"/>
     <col min="6" max="6" width="27.5" style="17" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" style="17" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" customWidth="1"/>
     <col min="9" max="9" width="23.5" customWidth="1"/>
     <col min="10" max="10" width="31.1640625" style="17" customWidth="1"/>
@@ -1924,644 +2135,740 @@
     <col min="12" max="12" width="20.6640625" customWidth="1"/>
     <col min="13" max="13" width="25.1640625" customWidth="1"/>
     <col min="14" max="14" width="27.5" style="17" customWidth="1"/>
-    <col min="15" max="15" width="25.1640625" customWidth="1"/>
+    <col min="15" max="15" width="25.1640625" style="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="54">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" ht="81">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="44" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="44" t="s">
         <v>169</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="44" t="s">
         <v>166</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="O1" s="13"/>
-    </row>
-    <row r="2" spans="1:15" ht="57">
-      <c r="A2" s="26">
+      <c r="O1" s="44" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="60">
+      <c r="A2" s="45">
         <v>200118941</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="30" t="s">
+      <c r="K2" s="48"/>
+      <c r="L2" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="M2" s="42" t="s">
+      <c r="M2" s="50" t="s">
         <v>209</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="N2" s="60" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="114">
-      <c r="A3" s="26">
+    <row r="3" spans="1:15" ht="120">
+      <c r="A3" s="45">
         <v>200057802</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="L3" s="30" t="s">
+      <c r="L3" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="M3" s="42" t="s">
+      <c r="M3" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="N3" s="35" t="s">
+      <c r="N3" s="60" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="114">
-      <c r="A4" s="26">
+    <row r="4" spans="1:15" ht="120">
+      <c r="A4" s="45">
         <v>200057802</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="M4" s="42" t="s">
+      <c r="M4" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="N4" s="35" t="s">
+      <c r="N4" s="60" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="133">
-      <c r="A5" s="26">
+    <row r="5" spans="1:15" ht="140">
+      <c r="A5" s="45">
         <v>200062105</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="L5" s="34" t="s">
+      <c r="L5" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="M5" s="42" t="s">
+      <c r="M5" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="N5" s="35" t="s">
+      <c r="N5" s="60" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="80">
-      <c r="A6" s="26">
+    <row r="6" spans="1:15" ht="100" customHeight="1">
+      <c r="A6" s="45">
         <v>200001829</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="46" t="s">
         <v>161</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30" t="s">
+      <c r="K6" s="49"/>
+      <c r="L6" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="M6" s="42" t="s">
+      <c r="M6" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="N6" s="35" t="s">
+      <c r="N6" s="60" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="133">
-      <c r="A7" s="26">
+    <row r="7" spans="1:15" ht="140">
+      <c r="A7" s="45">
         <v>200165953</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="45" t="s">
         <v>218</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="46" t="s">
         <v>171</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="46" t="s">
         <v>172</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="K7" s="36" t="s">
+      <c r="K7" s="53" t="s">
         <v>174</v>
       </c>
-      <c r="L7" s="30" t="s">
+      <c r="L7" s="49" t="s">
         <v>175</v>
       </c>
-      <c r="M7" s="42" t="s">
+      <c r="M7" s="50" t="s">
         <v>204</v>
       </c>
-      <c r="N7" s="35" t="s">
+      <c r="N7" s="60" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="120">
-      <c r="A8" s="26">
+      <c r="A8" s="45">
         <v>200169625</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="45" t="s">
         <v>184</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="41" t="s">
         <v>179</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="K8" s="36"/>
-      <c r="L8" s="30" t="s">
+      <c r="K8" s="53"/>
+      <c r="L8" s="49" t="s">
         <v>177</v>
       </c>
-      <c r="M8" s="42" t="s">
+      <c r="M8" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="N8" s="35" t="s">
+      <c r="N8" s="60" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="120">
-      <c r="A9" s="26">
+      <c r="A9" s="45">
         <v>200169625</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="45" t="s">
         <v>184</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="41" t="s">
         <v>179</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="K9" s="36"/>
-      <c r="L9" s="30" t="s">
+      <c r="K9" s="53"/>
+      <c r="L9" s="49" t="s">
         <v>177</v>
       </c>
-      <c r="M9" s="42" t="s">
+      <c r="M9" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="N9" s="35" t="s">
+      <c r="N9" s="60" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="120">
-      <c r="A10" s="26">
+      <c r="A10" s="45">
         <v>200169625</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="45" t="s">
         <v>184</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="41" t="s">
         <v>179</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="K10" s="36"/>
-      <c r="L10" s="30" t="s">
+      <c r="K10" s="53"/>
+      <c r="L10" s="49" t="s">
         <v>177</v>
       </c>
-      <c r="M10" s="42" t="s">
+      <c r="M10" s="50" t="s">
         <v>217</v>
       </c>
-      <c r="N10" s="17" t="s">
+      <c r="N10" s="57" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="108" customHeight="1">
-      <c r="A11" s="26">
+      <c r="A11" s="45">
         <v>200115342</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="45" t="s">
         <v>185</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="K11" s="36" t="s">
+      <c r="K11" s="53" t="s">
         <v>188</v>
       </c>
-      <c r="L11" s="30" t="s">
+      <c r="L11" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="M11" s="42" t="s">
+      <c r="M11" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="N11" s="35" t="s">
+      <c r="N11" s="60" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="91" customHeight="1">
-      <c r="A12" s="26">
+      <c r="A12" s="45">
         <v>200115342</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="45" t="s">
         <v>185</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="K12" s="36" t="s">
+      <c r="K12" s="53" t="s">
         <v>188</v>
       </c>
-      <c r="L12" s="30" t="s">
+      <c r="L12" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="M12" s="42" t="s">
+      <c r="M12" s="50" t="s">
         <v>206</v>
       </c>
-      <c r="N12" s="35" t="s">
+      <c r="N12" s="60" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="21" customHeight="1">
-      <c r="A13" s="26"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="26"/>
-    </row>
-    <row r="14" spans="1:15" ht="21" customHeight="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="26"/>
-    </row>
-    <row r="15" spans="1:15" ht="21" customHeight="1">
-      <c r="A15" s="26"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="26"/>
+    <row r="13" spans="1:15" ht="194" customHeight="1">
+      <c r="A13" s="61">
+        <v>200053987</v>
+      </c>
+      <c r="B13" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>237</v>
+      </c>
+      <c r="G13" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="H13" s="46" t="s">
+        <v>239</v>
+      </c>
+      <c r="I13" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="J13" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="K13" s="49" t="s">
+        <v>232</v>
+      </c>
+      <c r="L13" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="M13" s="62" t="s">
+        <v>235</v>
+      </c>
+      <c r="N13" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="O13" s="59" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="193" customHeight="1">
+      <c r="A14" s="61">
+        <v>200053987</v>
+      </c>
+      <c r="B14" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>225</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="E14" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>237</v>
+      </c>
+      <c r="G14" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="H14" s="46" t="s">
+        <v>239</v>
+      </c>
+      <c r="I14" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="J14" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="K14" s="49" t="s">
+        <v>232</v>
+      </c>
+      <c r="L14" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="M14" s="62" t="s">
+        <v>234</v>
+      </c>
+      <c r="N14" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="O14" s="59" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="193" customHeight="1">
+      <c r="A15" s="61">
+        <v>200053987</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>237</v>
+      </c>
+      <c r="G15" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="H15" s="46" t="s">
+        <v>239</v>
+      </c>
+      <c r="I15" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="J15" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="K15" s="49" t="s">
+        <v>232</v>
+      </c>
+      <c r="L15" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="M15" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="N15" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="O15" s="59" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="16" spans="1:15" ht="21" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="26"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="35"/>
     </row>
     <row r="17" spans="1:14" ht="21" customHeight="1">
       <c r="A17" s="26"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="28"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="26"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
       <c r="L17" s="16"/>
-      <c r="M17" s="35"/>
+      <c r="M17" s="30"/>
       <c r="N17" s="26"/>
     </row>
     <row r="18" spans="1:14" ht="21" customHeight="1">
       <c r="A18" s="26"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="28"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="27"/>
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="26"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
       <c r="L18" s="16"/>
-      <c r="M18" s="35"/>
+      <c r="M18" s="30"/>
       <c r="N18" s="26"/>
     </row>
     <row r="19" spans="1:14" ht="21" customHeight="1">
       <c r="A19" s="26"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="40"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="26"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
       <c r="L19" s="16"/>
-      <c r="M19" s="35"/>
+      <c r="M19" s="30"/>
       <c r="N19" s="26"/>
     </row>
     <row r="24" spans="1:14">
       <c r="C24"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="23" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" xr:uid="{4463D349-9552-F040-A639-07677033794F}"/>
     <hyperlink ref="K7" r:id="rId2" tooltip="Link to PubMed record" display="https://www.ncbi.nlm.nih.gov/pubmed/35884972" xr:uid="{D886AF7C-B7E0-6347-95AB-45140B3EEF79}"/>
@@ -2576,6 +2883,9 @@
     <hyperlink ref="L4" r:id="rId11" xr:uid="{8C0E6DA6-2F49-384A-BE04-8B74A927E255}"/>
     <hyperlink ref="L9" r:id="rId12" xr:uid="{5149B4B3-D738-A84E-B926-C59E340E79EB}"/>
     <hyperlink ref="L10" r:id="rId13" xr:uid="{9E462C14-E3D6-6D45-94BD-1831EBE2B53D}"/>
+    <hyperlink ref="L13" r:id="rId14" xr:uid="{1F30C8E0-E145-1549-BC95-16CFE6C9D924}"/>
+    <hyperlink ref="L14" r:id="rId15" xr:uid="{F883605B-9E52-F24E-8FCA-90384291420F}"/>
+    <hyperlink ref="L15" r:id="rId16" xr:uid="{5D4E696B-4080-0449-96B8-7BA662794F89}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3397,6 +3707,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010034B2111F16753748B07B8B2A03D6410C" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c54d6f00b4000a0e053db110112d707">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dba05a22-d3d4-4800-8353-2deabbd0fb1d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca2460e8561fc9eb4be35c86fe727f91" ns3:_="">
     <xsd:import namespace="dba05a22-d3d4-4800-8353-2deabbd0fb1d"/>
@@ -3560,7 +3876,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3569,13 +3885,16 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F26D0B6-AFD8-4D33-AA54-AAEB31DB979E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{833422F9-EA10-412F-A3DB-70A7B71D2D3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3593,19 +3912,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2B9A09B-0EA7-4ECB-B6A7-B701DD5D6BD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F26D0B6-AFD8-4D33-AA54-AAEB31DB979E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>